<commit_message>
criando arquivos de exemplo do ledger
</commit_message>
<xml_diff>
--- a/temp-contas.xlsx
+++ b/temp-contas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="460" windowWidth="24560" windowHeight="14240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3520" yWindow="2860" windowWidth="24560" windowHeight="14240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="214">
   <si>
     <t>RECEITAS</t>
   </si>
@@ -634,6 +634,42 @@
   </si>
   <si>
     <t>Superávit ou déficit acumulado</t>
+  </si>
+  <si>
+    <t>Contribuições</t>
+  </si>
+  <si>
+    <t>Doaçoes</t>
+  </si>
+  <si>
+    <t>Nome Completo - CPF</t>
+  </si>
+  <si>
+    <t>Banco/Conta</t>
+  </si>
+  <si>
+    <t>Receita</t>
+  </si>
+  <si>
+    <t>Ativo</t>
+  </si>
+  <si>
+    <t>Despesa</t>
+  </si>
+  <si>
+    <t>Transporte e Viagens</t>
+  </si>
+  <si>
+    <t>Propaganda Institucional</t>
+  </si>
+  <si>
+    <t>Venda de Material para Divulgação</t>
+  </si>
+  <si>
+    <t>Material para Comercialização</t>
+  </si>
+  <si>
+    <t>Despesas com alistamento</t>
   </si>
 </sst>
 </file>
@@ -983,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1737,165 +1773,254 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>206</v>
+      </c>
+      <c r="I9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>207</v>
+      </c>
+      <c r="I11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>208</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>143</v>
+      </c>
+      <c r="I16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>208</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>208</v>
+      </c>
+      <c r="I18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>208</v>
+      </c>
+      <c r="I19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>208</v>
+      </c>
+      <c r="I20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>208</v>
+      </c>
+      <c r="I21" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>208</v>
+      </c>
+      <c r="I22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>208</v>
+      </c>
+      <c r="I23" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>139</v>
       </c>

</xml_diff>